<commit_message>
mengisi bab 1 dan bab 2 pada laporan pkl
</commit_message>
<xml_diff>
--- a/Excel Pak Madi1.xlsx
+++ b/Excel Pak Madi1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRAKERIN\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD2E9F5-AECE-4220-83C1-EBE234D06E8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22682857-8B3E-44A4-9A8B-C7AF72321C4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="6" xr2:uid="{4F68D828-C374-4000-835B-2E94470A6855}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{4F68D828-C374-4000-835B-2E94470A6855}"/>
   </bookViews>
   <sheets>
     <sheet name="ALOKASI Waktu" sheetId="1" r:id="rId1"/>
@@ -585,6 +585,19 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -606,34 +619,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -964,41 +964,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="43"/>
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
@@ -1038,45 +1038,45 @@
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
-      <c r="X3" s="33"/>
-      <c r="Y3" s="33"/>
-      <c r="Z3" s="33"/>
-      <c r="AA3" s="33"/>
-      <c r="AB3" s="33"/>
-      <c r="AC3" s="33"/>
-      <c r="AD3" s="33"/>
-      <c r="AE3" s="33"/>
-      <c r="AF3" s="33"/>
-      <c r="AG3" s="33"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="44"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="44"/>
+      <c r="X3" s="44"/>
+      <c r="Y3" s="44"/>
+      <c r="Z3" s="44"/>
+      <c r="AA3" s="44"/>
+      <c r="AB3" s="44"/>
+      <c r="AC3" s="44"/>
+      <c r="AD3" s="44"/>
+      <c r="AE3" s="44"/>
+      <c r="AF3" s="44"/>
+      <c r="AG3" s="44"/>
     </row>
     <row r="4" spans="1:33" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="45" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="7">
@@ -1162,8 +1162,8 @@
       </c>
     </row>
     <row r="5" spans="1:33" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
-      <c r="B5" s="34"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="8">
         <v>20</v>
       </c>
@@ -1259,8 +1259,8 @@
       </c>
     </row>
     <row r="6" spans="1:33" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -1928,37 +1928,37 @@
         <f>SUM(B8:B18)</f>
         <v>201</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="37"/>
-      <c r="T20" s="37"/>
-      <c r="U20" s="37"/>
-      <c r="V20" s="37"/>
-      <c r="W20" s="37"/>
-      <c r="X20" s="37"/>
-      <c r="Y20" s="37"/>
-      <c r="Z20" s="37"/>
-      <c r="AA20" s="37"/>
-      <c r="AB20" s="37"/>
-      <c r="AC20" s="37"/>
-      <c r="AD20" s="37"/>
-      <c r="AE20" s="37"/>
-      <c r="AF20" s="37"/>
-      <c r="AG20" s="38"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+      <c r="R20" s="48"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="48"/>
+      <c r="V20" s="48"/>
+      <c r="W20" s="48"/>
+      <c r="X20" s="48"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="48"/>
+      <c r="AA20" s="48"/>
+      <c r="AB20" s="48"/>
+      <c r="AC20" s="48"/>
+      <c r="AD20" s="48"/>
+      <c r="AE20" s="48"/>
+      <c r="AF20" s="48"/>
+      <c r="AG20" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1990,31 +1990,31 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="34" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2040,13 +2040,13 @@
         <f>E4+1000</f>
         <v>8000</v>
       </c>
-      <c r="H4" s="44" t="s">
+      <c r="H4" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="44" t="s">
+      <c r="I4" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="44" t="s">
+      <c r="J4" s="33" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2072,13 +2072,13 @@
         <f t="shared" ref="F5" si="2">E5+1000</f>
         <v>8000</v>
       </c>
-      <c r="H5" s="44" t="s">
+      <c r="H5" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="44" t="s">
+      <c r="I5" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="44" t="s">
+      <c r="J5" s="33" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2104,13 +2104,13 @@
         <f t="shared" ref="F6" si="3">E6+1000</f>
         <v>16000</v>
       </c>
-      <c r="H6" s="44" t="s">
+      <c r="H6" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="44" t="s">
+      <c r="I6" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="44" t="s">
+      <c r="J6" s="33" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2136,13 +2136,13 @@
         <f t="shared" ref="F7" si="4">E7+1000</f>
         <v>18000</v>
       </c>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="I7" s="44" t="s">
+      <c r="I7" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="44" t="s">
+      <c r="J7" s="33" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2168,13 +2168,13 @@
         <f t="shared" ref="F8" si="5">E8+1000</f>
         <v>8000</v>
       </c>
-      <c r="H8" s="44" t="s">
+      <c r="H8" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="44" t="s">
+      <c r="I8" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="J8" s="44" t="s">
+      <c r="J8" s="33" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2200,13 +2200,13 @@
         <f t="shared" ref="F9" si="6">E9+1000</f>
         <v>13000</v>
       </c>
-      <c r="H9" s="44" t="s">
+      <c r="H9" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="I9" s="44" t="s">
+      <c r="I9" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="44" t="s">
+      <c r="J9" s="33" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2303,128 +2303,128 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="48" t="s">
+      <c r="A16" s="52"/>
+      <c r="B16" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="48" t="s">
+      <c r="D16" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="48" t="s">
+      <c r="E16" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="48" t="s">
+      <c r="F16" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="G16" s="48" t="s">
+      <c r="G16" s="36" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="48" t="s">
+      <c r="E17" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="G17" s="48" t="s">
+      <c r="G17" s="36" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="48" t="s">
+      <c r="D18" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="48" t="s">
+      <c r="E18" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="48" t="s">
+      <c r="F18" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="48" t="s">
+      <c r="G18" s="36" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="48" t="s">
+      <c r="D20" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="48" t="s">
+      <c r="E20" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="48" t="s">
+      <c r="F20" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="G20" s="48" t="s">
+      <c r="G20" s="36" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="48" t="s">
+      <c r="B21" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="48" t="s">
+      <c r="D21" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="48" t="s">
+      <c r="E21" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="48" t="s">
+      <c r="F21" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="48" t="s">
+      <c r="G21" s="36" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2444,7 +2444,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2454,30 +2454,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="38" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2701,8 +2701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51DCE48-217C-4310-8196-483624757B37}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2713,14 +2713,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
@@ -2965,32 +2965,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="38" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3207,7 +3207,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3218,14 +3218,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
@@ -3452,6 +3452,7 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3459,14 +3460,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85573BF8-F4D2-44FD-AFF8-C2222E067CD4}">
   <dimension ref="A3:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
     <col min="2" max="5" width="14.140625" customWidth="1"/>
+    <col min="8" max="10" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3485,13 +3487,13 @@
       <c r="E3" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="I3" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="52" t="s">
+      <c r="J3" s="40" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3502,303 +3504,303 @@
       <c r="B4" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="H4" s="51" t="s">
+      <c r="H4" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="51" t="s">
+      <c r="I4" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="51" t="s">
+      <c r="J4" s="39" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="47">
+      <c r="A5" s="35">
         <v>2</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="53"/>
-      <c r="H5" s="51" t="s">
+      <c r="D5" s="41"/>
+      <c r="H5" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="51" t="s">
+      <c r="I5" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="51" t="s">
+      <c r="J5" s="39" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="47">
+      <c r="A6" s="35">
         <v>3</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="H6" s="51" t="s">
+      <c r="D6" s="41"/>
+      <c r="H6" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="51" t="s">
+      <c r="I6" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="51" t="s">
+      <c r="J6" s="39" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="47">
+      <c r="A7" s="35">
         <v>4</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="H7" s="51" t="s">
+      <c r="D7" s="41"/>
+      <c r="H7" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="I7" s="51" t="s">
+      <c r="I7" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="51" t="s">
+      <c r="J7" s="39" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="47">
+      <c r="A8" s="35">
         <v>5</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="53"/>
-      <c r="H8" s="51" t="s">
+      <c r="D8" s="41"/>
+      <c r="H8" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="51" t="s">
+      <c r="I8" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="J8" s="51" t="s">
+      <c r="J8" s="39" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="47">
+      <c r="A9" s="35">
         <v>6</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="53"/>
-      <c r="H9" s="51" t="s">
+      <c r="D9" s="41"/>
+      <c r="H9" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="I9" s="51" t="s">
+      <c r="I9" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="51" t="s">
+      <c r="J9" s="39" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="47">
+      <c r="A10" s="35">
         <v>7</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="53"/>
+      <c r="D10" s="41"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="47">
+      <c r="A11" s="35">
         <v>8</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="53"/>
+      <c r="D11" s="41"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="47">
+      <c r="A12" s="35">
         <v>9</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="53"/>
+      <c r="D12" s="41"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="47">
+      <c r="A13" s="35">
         <v>10</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="53"/>
+      <c r="D13" s="41"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="47">
+      <c r="A14" s="35">
         <v>11</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="53"/>
+      <c r="D14" s="41"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="47">
+      <c r="A15" s="35">
         <v>12</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="54" t="s">
+      <c r="C15" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="53"/>
+      <c r="D15" s="41"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="47">
+      <c r="A16" s="35">
         <v>13</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="53"/>
+      <c r="D16" s="41"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="47">
+      <c r="A17" s="35">
         <v>14</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="53"/>
+      <c r="D17" s="41"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="47">
+      <c r="A18" s="35">
         <v>15</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="53"/>
+      <c r="D18" s="41"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="47">
+      <c r="A19" s="35">
         <v>16</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="54" t="s">
+      <c r="C19" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="53"/>
+      <c r="D19" s="41"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="47">
+      <c r="A20" s="35">
         <v>17</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="53"/>
+      <c r="D20" s="41"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="47">
+      <c r="A21" s="35">
         <v>18</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="53"/>
+      <c r="D21" s="41"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="47">
+      <c r="A22" s="35">
         <v>19</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="54" t="s">
+      <c r="C22" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="53"/>
+      <c r="D22" s="41"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="47">
+      <c r="A23" s="35">
         <v>20</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="53"/>
+      <c r="D23" s="41"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="47">
+      <c r="A24" s="35">
         <v>21</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="54" t="s">
+      <c r="C24" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="53"/>
+      <c r="D24" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>